<commit_message>
added spacer to BOM
</commit_message>
<xml_diff>
--- a/uac BOM.xlsx
+++ b/uac BOM.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="107">
   <si>
     <t>Part</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>490-1198-1-ND</t>
+  </si>
+  <si>
+    <t>spacers m3x40</t>
   </si>
 </sst>
 </file>
@@ -725,11 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I67" sqref="I67"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -816,7 +819,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J66" si="0">B3*I3</f>
+        <f t="shared" ref="J3:J67" si="0">B3*I3</f>
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
@@ -2224,12 +2227,30 @@
       </c>
     </row>
     <row r="67" spans="2:10">
-      <c r="I67" s="1" t="s">
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>106</v>
+      </c>
+      <c r="H67">
+        <v>1466833</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="I68" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J67" s="3">
-        <f>SUM(J2:J66)</f>
-        <v>62.538699999999999</v>
+      <c r="J68" s="3">
+        <f>SUM(J2:J67)</f>
+        <v>64.458699999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>